<commit_message>
[Add] XlsxToJson 변환 데이터 추가
</commit_message>
<xml_diff>
--- a/Assets/Data/Xlsx/PlayerData.xlsx
+++ b/Assets/Data/Xlsx/PlayerData.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuwonCha\SpartaCodingUnity\CampWeek9\TeamProject_ONE-PICKAXE\Assets\Data\Xlsx\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D86ABA6-CA67-4BD5-B41F-E00A5205211A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="PlayerData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="NBPjzc2P+45+eJoqf/RhIqRupmPxcXwYLIAWSOjqspI="/>
@@ -45,16 +54,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Malgun Gothic"/>
     </font>
@@ -64,7 +73,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -74,7 +83,13 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -88,41 +103,41 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -312,28 +327,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="9.88"/>
-    <col customWidth="1" min="2" max="2" width="12.38"/>
-    <col customWidth="1" min="3" max="3" width="12.5"/>
-    <col customWidth="1" min="4" max="4" width="12.63"/>
-    <col customWidth="1" min="5" max="5" width="15.13"/>
-    <col customWidth="1" min="6" max="26" width="7.63"/>
+    <col min="1" max="1" width="9.90625" customWidth="1"/>
+    <col min="2" max="2" width="12.36328125" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" customWidth="1"/>
+    <col min="5" max="5" width="15.08984375" customWidth="1"/>
+    <col min="6" max="26" width="7.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.5" customHeight="1">
+    <row r="1" spans="1:5" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -346,41 +361,41 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="16.5" customHeight="1">
-      <c r="A2" s="3">
-        <v>5.0</v>
-      </c>
-      <c r="B2" s="3">
-        <v>10.0</v>
-      </c>
-      <c r="C2" s="3" t="s">
+    <row r="2" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A2" s="2">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="B2" s="2">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" ht="16.5" customHeight="1"/>
-    <row r="4" ht="16.5" customHeight="1"/>
-    <row r="5" ht="16.5" customHeight="1"/>
-    <row r="6" ht="16.5" customHeight="1"/>
-    <row r="7" ht="16.5" customHeight="1"/>
-    <row r="8" ht="16.5" customHeight="1"/>
-    <row r="9" ht="16.5" customHeight="1"/>
-    <row r="10" ht="16.5" customHeight="1"/>
-    <row r="11" ht="16.5" customHeight="1"/>
-    <row r="12" ht="16.5" customHeight="1"/>
-    <row r="13" ht="16.5" customHeight="1"/>
-    <row r="14" ht="16.5" customHeight="1"/>
-    <row r="15" ht="16.5" customHeight="1"/>
-    <row r="16" ht="16.5" customHeight="1"/>
+    <row r="3" spans="1:5" ht="16.5" customHeight="1"/>
+    <row r="4" spans="1:5" ht="16.5" customHeight="1"/>
+    <row r="5" spans="1:5" ht="16.5" customHeight="1"/>
+    <row r="6" spans="1:5" ht="16.5" customHeight="1"/>
+    <row r="7" spans="1:5" ht="16.5" customHeight="1"/>
+    <row r="8" spans="1:5" ht="16.5" customHeight="1"/>
+    <row r="9" spans="1:5" ht="16.5" customHeight="1"/>
+    <row r="10" spans="1:5" ht="16.5" customHeight="1"/>
+    <row r="11" spans="1:5" ht="16.5" customHeight="1"/>
+    <row r="12" spans="1:5" ht="16.5" customHeight="1"/>
+    <row r="13" spans="1:5" ht="16.5" customHeight="1"/>
+    <row r="14" spans="1:5" ht="16.5" customHeight="1"/>
+    <row r="15" spans="1:5" ht="16.5" customHeight="1"/>
+    <row r="16" spans="1:5" ht="16.5" customHeight="1"/>
     <row r="17" ht="16.5" customHeight="1"/>
     <row r="18" ht="16.5" customHeight="1"/>
     <row r="19" ht="16.5" customHeight="1"/>
@@ -1366,9 +1381,7 @@
     <row r="999" ht="16.5" customHeight="1"/>
     <row r="1000" ht="16.5" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>